<commit_message>
Starting 'modal' layout for data view and update.
</commit_message>
<xml_diff>
--- a/public/assets/Schema.xlsx
+++ b/public/assets/Schema.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_BootCamp\Projects\Group-Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_BootCamp\Projects\Group-Project-2\auto-tracker\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C51699D-3EFC-4BCD-950C-4B414EF17A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6584F3-9ACA-49DF-9748-E4554AA9FC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="1110" windowWidth="24060" windowHeight="14190" xr2:uid="{BEB72CD0-6CB0-4421-89C6-2148A3815F62}"/>
+    <workbookView xWindow="3975" yWindow="855" windowWidth="24570" windowHeight="14790" activeTab="1" xr2:uid="{BEB72CD0-6CB0-4421-89C6-2148A3815F62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Auto-Tracker Application</t>
   </si>
@@ -112,13 +113,25 @@
   </si>
   <si>
     <t>Year (i.e. 2018)</t>
+  </si>
+  <si>
+    <t>Driver Modal</t>
+  </si>
+  <si>
+    <t>[Update]     [Delete]</t>
+  </si>
+  <si>
+    <t>Vehicle Modal</t>
+  </si>
+  <si>
+    <t>Purchase Mileage (i.e. 25000)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +170,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -172,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -219,16 +247,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -237,6 +275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5D7CC2-6ACA-471E-BF2E-C1FE68612F6B}">
   <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,15 +731,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -702,144 +748,144 @@
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="8"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="8"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -850,4 +896,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3A6073-9BD5-4E11-862D-58E4A4CC6E21}">
+  <dimension ref="C3:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>